<commit_message>
added synthetic image to xl sheet
</commit_message>
<xml_diff>
--- a/latex/data/Rank2Scalabilityv2.xlsx
+++ b/latex/data/Rank2Scalabilityv2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rnu/Documents/research/lawton/planc/latex/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E4912C-DB97-924B-9B5E-B60A2A1DDCC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC04EC5-76BE-684F-B089-A7D36766AD72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="460" windowWidth="27440" windowHeight="17040" activeTab="3" xr2:uid="{8722A55B-31FB-6E49-B1FD-EE37D33A2388}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>Reuters</t>
   </si>
@@ -77,7 +77,13 @@
     <t>PUBMED</t>
   </si>
   <si>
-    <t>PUBMED Speedup</t>
+    <t>PUBMED level 6</t>
+  </si>
+  <si>
+    <t>PUBMED level 6 Speedup</t>
+  </si>
+  <si>
+    <t>PUBMED level 1 Speedup</t>
   </si>
 </sst>
 </file>
@@ -3198,36 +3204,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3243,7 +3219,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PUBMED Speedup</c:v>
+                  <c:v>PUBMED level 1 Speedup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3408,6 +3384,111 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2239-2D49-A411-060AD58C4C4A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>speedup!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PUBMED level 6 Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>speedup!$J$2:$J$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0610687112586261</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1024332549143203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1305163984501378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1491733932239589</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1311628423353186</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1126696876842559</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1375297538534377</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1196926426726559</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9228882359703472</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.564436034981286</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4906301472195396</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5801222842676923</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6072245392946765</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5408174317744758</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.3851484281959108</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5445446751806342</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2363527130548735</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.547777637916159</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4451144788510262</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2187776616491868</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2239-2D49-A411-060AD58C4C4A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3538,6 +3619,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -10386,8 +10498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EA2AA6-1F46-994A-8279-79EB37F52A30}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10412,7 +10524,13 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
       </c>
       <c r="N1" t="s">
         <v>5</v>
@@ -10454,6 +10572,13 @@
         <f>G$2/G2</f>
         <v>1</v>
       </c>
+      <c r="I2">
+        <v>451.564719999999</v>
+      </c>
+      <c r="J2">
+        <f>I$2/I2</f>
+        <v>1</v>
+      </c>
       <c r="N2">
         <v>4.2987599999999997</v>
       </c>
@@ -10494,6 +10619,13 @@
         <f t="shared" ref="H3:H22" si="1">G$2/G3</f>
         <v>1.1177896542436314</v>
       </c>
+      <c r="I3">
+        <v>425.57537999999897</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J22" si="2">I$2/I3</f>
+        <v>1.0610687112586261</v>
+      </c>
       <c r="N3">
         <v>4.6227799999999997</v>
       </c>
@@ -10534,6 +10666,13 @@
         <f t="shared" si="1"/>
         <v>1.1406376576785096</v>
       </c>
+      <c r="I4">
+        <v>409.60730999999998</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>1.1024332549143203</v>
+      </c>
       <c r="N4">
         <v>4.58324</v>
       </c>
@@ -10574,6 +10713,13 @@
         <f t="shared" si="1"/>
         <v>1.20535891721011</v>
       </c>
+      <c r="I5">
+        <v>399.43225999999999</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>1.1305163984501378</v>
+      </c>
       <c r="N5">
         <v>3.9264000000000001</v>
       </c>
@@ -10614,6 +10760,13 @@
         <f t="shared" si="1"/>
         <v>1.2071304129503584</v>
       </c>
+      <c r="I6">
+        <v>392.947419999999</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>1.1491733932239589</v>
+      </c>
       <c r="O6">
         <v>4.9314999999999998</v>
       </c>
@@ -10648,6 +10801,13 @@
         <f t="shared" si="1"/>
         <v>1.1601662046600867</v>
       </c>
+      <c r="I7">
+        <v>399.20398999999901</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>1.1311628423353186</v>
+      </c>
       <c r="O7">
         <v>4.2575900000000004</v>
       </c>
@@ -10682,6 +10842,13 @@
         <f t="shared" si="1"/>
         <v>1.1856465344837437</v>
       </c>
+      <c r="I8">
+        <v>405.83896999999899</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>1.1126696876842559</v>
+      </c>
       <c r="O8">
         <v>4.6992700000000003</v>
       </c>
@@ -10716,6 +10883,13 @@
         <f t="shared" si="1"/>
         <v>1.2453368964025004</v>
       </c>
+      <c r="I9">
+        <v>396.96958999999902</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>1.1375297538534377</v>
+      </c>
       <c r="O9">
         <v>3.9377499999999999</v>
       </c>
@@ -10750,6 +10924,13 @@
         <f t="shared" si="1"/>
         <v>1.2210607820363919</v>
       </c>
+      <c r="I10">
+        <v>403.29345999999998</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>1.1196926426726559</v>
+      </c>
       <c r="O10">
         <v>3.8122699999999998</v>
       </c>
@@ -10784,6 +10965,13 @@
         <f t="shared" si="1"/>
         <v>4.6548888434977371</v>
       </c>
+      <c r="I11">
+        <v>154.492639999999</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>2.9228882359703472</v>
+      </c>
       <c r="O11">
         <v>3.6942599999999999</v>
       </c>
@@ -10818,6 +11006,13 @@
         <f t="shared" si="1"/>
         <v>4.2098642699182367</v>
       </c>
+      <c r="I12">
+        <v>176.08733999999899</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>2.564436034981286</v>
+      </c>
       <c r="O12">
         <v>3.5505499999999999</v>
       </c>
@@ -10852,6 +11047,13 @@
         <f t="shared" si="1"/>
         <v>4.193818784478669</v>
       </c>
+      <c r="I13">
+        <v>181.30540999999999</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>2.4906301472195396</v>
+      </c>
       <c r="O13">
         <v>3.3760300000000001</v>
       </c>
@@ -10886,6 +11088,13 @@
         <f t="shared" si="1"/>
         <v>3.910705960540803</v>
       </c>
+      <c r="I14">
+        <v>175.01678999999999</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>2.5801222842676923</v>
+      </c>
       <c r="O14">
         <v>3.4249900000000002</v>
       </c>
@@ -10920,6 +11129,13 @@
         <f t="shared" si="1"/>
         <v>4.4129416439536824</v>
       </c>
+      <c r="I15">
+        <v>173.19748000000001</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>2.6072245392946765</v>
+      </c>
       <c r="O15">
         <v>3.1164800000000001</v>
       </c>
@@ -10954,6 +11170,13 @@
         <f t="shared" si="1"/>
         <v>4.4602553630540385</v>
       </c>
+      <c r="I16">
+        <v>177.72418999999999</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>2.5408174317744758</v>
+      </c>
       <c r="O16">
         <v>2.2753100000000002</v>
       </c>
@@ -10988,6 +11211,13 @@
         <f t="shared" si="1"/>
         <v>4.3962942891105712</v>
       </c>
+      <c r="I17">
+        <v>189.32352999999901</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>2.3851484281959108</v>
+      </c>
       <c r="O17">
         <v>2.4762</v>
       </c>
@@ -11022,6 +11252,13 @@
         <f t="shared" si="1"/>
         <v>4.2390513126812417</v>
       </c>
+      <c r="I18">
+        <v>177.46385999999899</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>2.5445446751806342</v>
+      </c>
       <c r="O18">
         <v>2.6131899999999999</v>
       </c>
@@ -11056,6 +11293,13 @@
         <f t="shared" si="1"/>
         <v>4.2649978093543268</v>
       </c>
+      <c r="I19">
+        <v>201.92016999999899</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>2.2363527130548735</v>
+      </c>
       <c r="O19">
         <v>2.4928400000000002</v>
       </c>
@@ -11090,6 +11334,13 @@
         <f t="shared" si="1"/>
         <v>4.0676241876358672</v>
       </c>
+      <c r="I20">
+        <v>177.23866999999899</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>2.547777637916159</v>
+      </c>
       <c r="O20">
         <v>2.8723399999999999</v>
       </c>
@@ -11124,6 +11375,13 @@
         <f t="shared" si="1"/>
         <v>4.5390333844898034</v>
       </c>
+      <c r="I21">
+        <v>184.68039999999999</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>2.4451144788510262</v>
+      </c>
       <c r="O21">
         <v>2.9455100000000001</v>
       </c>
@@ -11157,6 +11415,13 @@
       <c r="H22">
         <f t="shared" si="1"/>
         <v>3.6984399478419121</v>
+      </c>
+      <c r="I22">
+        <v>203.519589999999</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>2.2187776616491868</v>
       </c>
       <c r="O22">
         <v>2.84904</v>

</xml_diff>